<commit_message>
documento ecxel de diccionarios de bd
</commit_message>
<xml_diff>
--- a/assets/docs/AdminVentas v.2 - DB_DICTIONARY.xlsx
+++ b/assets/docs/AdminVentas v.2 - DB_DICTIONARY.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\adminventas_ci\assets\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="21315" windowHeight="9285" activeTab="1"/>
   </bookViews>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="128">
   <si>
     <t>av_administracion_entidades</t>
   </si>
@@ -230,9 +235,6 @@
     <t>Catálogo de entidades (estados)</t>
   </si>
   <si>
-    <t>Catalogo de formas de pago</t>
-  </si>
-  <si>
     <t>Catálogo de almacenes</t>
   </si>
   <si>
@@ -242,9 +244,6 @@
     <t>Catálogo de pasillos por almacen</t>
   </si>
   <si>
-    <t>Catalogo de tipos de almacen</t>
-  </si>
-  <si>
     <t>Catálogo de árticulos</t>
   </si>
   <si>
@@ -384,13 +383,37 @@
   </si>
   <si>
     <t>id_personal, id_clave, id_nivel, id_empresa, id_sucursal, id_perfil</t>
+  </si>
+  <si>
+    <t>av_administracion_descuentos</t>
+  </si>
+  <si>
+    <t>id_administracion_descuentos</t>
+  </si>
+  <si>
+    <t>Catálogo de descuentos</t>
+  </si>
+  <si>
+    <t>av_administracion_impuestos</t>
+  </si>
+  <si>
+    <t>id_administracion_impuestos</t>
+  </si>
+  <si>
+    <t>Catálogo de impuestos</t>
+  </si>
+  <si>
+    <t>Catálogo de formas de pago</t>
+  </si>
+  <si>
+    <t>Catálogo de tipos de almacen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +437,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -429,7 +478,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -573,7 +622,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="hair">
         <color indexed="64"/>
       </left>
       <right style="hair">
@@ -591,13 +640,26 @@
       <left style="hair">
         <color indexed="64"/>
       </left>
-      <right style="hair">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="hair">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -606,22 +668,29 @@
       <left style="hair">
         <color indexed="64"/>
       </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -662,30 +731,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,6 +790,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -743,7 +841,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -778,7 +876,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -987,18 +1085,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="19" customWidth="1"/>
     <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="32.5703125" customWidth="1"/>
     <col min="10" max="10" width="69.7109375" bestFit="1" customWidth="1"/>
@@ -1043,83 +1141,81 @@
       <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>34</v>
+      <c r="C2" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>56</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="22"/>
+      <c r="J3" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="16" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="19" t="s">
+      <c r="D4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="10" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1129,49 +1225,48 @@
       <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="C5" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10" t="s">
-        <v>72</v>
+      <c r="F5" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="C6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="I6" s="9"/>
       <c r="J6" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1181,51 +1276,49 @@
       <c r="B7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="19" t="s">
+      <c r="C7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="21">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="19" t="s">
+      <c r="C8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="I8" s="9"/>
       <c r="J8" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1235,53 +1328,51 @@
       <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>34</v>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>91</v>
-      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="10" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="21">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="19" t="s">
+      <c r="C10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10" t="s">
-        <v>82</v>
+      <c r="I10" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1291,51 +1382,53 @@
       <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="19" t="s">
+      <c r="C11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>11</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1345,57 +1438,51 @@
       <c r="B13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="19" t="s">
+      <c r="C13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>13</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>34</v>
-      </c>
       <c r="F14" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1405,53 +1492,57 @@
       <c r="B15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>36</v>
+      <c r="C15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="J15" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="21">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="19" t="s">
+      <c r="C16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>65</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G16" s="9"/>
       <c r="H16" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1461,55 +1552,53 @@
       <c r="B17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="19" t="s">
+      <c r="C17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>17</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>36</v>
-      </c>
       <c r="F18" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="I18" s="9"/>
       <c r="J18" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1519,53 +1608,55 @@
       <c r="B19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="19" t="s">
+      <c r="C19" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="17" t="s">
         <v>34</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="I19" s="9" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="21">
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>34</v>
+      <c r="C20" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
-      <c r="I20" s="9" t="s">
-        <v>0</v>
-      </c>
+      <c r="I20" s="9"/>
       <c r="J20" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1575,45 +1666,53 @@
       <c r="B21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="19"/>
+      <c r="C21" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="F21" s="9" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="I21" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="J21" s="10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="21">
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="19"/>
+      <c r="C22" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="F22" s="9" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
+      <c r="I22" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="J22" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1623,57 +1722,116 @@
       <c r="B23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="19" t="s">
+      <c r="C23" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="19"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
+      <c r="A24" s="21">
         <v>23</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="17"/>
+      <c r="F25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <v>25</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="14" t="s">
-        <v>93</v>
-      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1685,7 +1843,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1721,19 +1879,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1741,19 +1899,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1761,19 +1919,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
         <v>97</v>
       </c>
-      <c r="C4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="19" t="s">
+      <c r="D4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1781,22 +1939,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1804,19 +1962,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1824,19 +1982,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1844,22 +2002,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1867,19 +2025,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1887,22 +2045,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1910,22 +2068,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1933,15 +2091,18 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="19"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>